<commit_message>
add 2 phase model
</commit_message>
<xml_diff>
--- a/Analysis/Fig Data/fig1.xlsx
+++ b/Analysis/Fig Data/fig1.xlsx
@@ -38,7 +38,7 @@
     <t xml:space="preserve">CN</t>
   </si>
   <si>
-    <t xml:space="preserve">2015 Jan. to 2019 Dec.</t>
+    <t xml:space="preserve">2015 Jan to 2019 Dec</t>
   </si>
   <si>
     <t xml:space="preserve">AU</t>
@@ -50,10 +50,10 @@
     <t xml:space="preserve">UK</t>
   </si>
   <si>
-    <t xml:space="preserve">2020 Jan. to 2023 Jun.</t>
+    <t xml:space="preserve">2020 Jan to 2023 Jun</t>
   </si>
   <si>
-    <t xml:space="preserve">2023 Jun. onwards</t>
+    <t xml:space="preserve">2023 Jun onwards</t>
   </si>
 </sst>
 </file>

</xml_diff>